<commit_message>
llamadas a mis funciones
</commit_message>
<xml_diff>
--- a/build/classes/Excel/Yañez_Gonzalez_Christian_Emmanuel.xlsx
+++ b/build/classes/Excel/Yañez_Gonzalez_Christian_Emmanuel.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="127">
   <si>
     <t>Estado</t>
   </si>
@@ -73,6 +73,15 @@
     <t>x</t>
   </si>
   <si>
+    <t>-47</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
     <t>-50</t>
   </si>
   <si>
@@ -91,57 +100,39 @@
     <t>{</t>
   </si>
   <si>
+    <t>-92</t>
+  </si>
+  <si>
+    <t>return</t>
+  </si>
+  <si>
     <t>3</t>
   </si>
   <si>
+    <t>-19</t>
+  </si>
+  <si>
+    <t>-54</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
     <t>-55</t>
   </si>
   <si>
     <t>=</t>
   </si>
   <si>
-    <t>-19</t>
-  </si>
-  <si>
-    <t>-24</t>
-  </si>
-  <si>
-    <t>+</t>
-  </si>
-  <si>
-    <t>-25</t>
-  </si>
-  <si>
-    <t>*</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>-27</t>
-  </si>
-  <si>
-    <t>/</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>-92</t>
-  </si>
-  <si>
-    <t>return</t>
-  </si>
-  <si>
-    <t>-54</t>
-  </si>
-  <si>
-    <t>}</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
     <t>8</t>
   </si>
   <si>
@@ -217,13 +208,7 @@
     <t>0</t>
   </si>
   <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>10</t>
+    <t>14</t>
   </si>
   <si>
     <t>Ambito</t>
@@ -295,10 +280,7 @@
     <t>Errores</t>
   </si>
   <si>
-    <t>a -&gt;  TE4</t>
-  </si>
-  <si>
-    <t>x -&gt;  TE1</t>
+    <t xml:space="preserve">a -&gt; </t>
   </si>
   <si>
     <t>Regla</t>
@@ -319,12 +301,12 @@
     <t/>
   </si>
   <si>
+    <t>Acept</t>
+  </si>
+  <si>
     <t>id</t>
   </si>
   <si>
-    <t>Acept</t>
-  </si>
-  <si>
     <t>Entradas</t>
   </si>
   <si>
@@ -352,25 +334,16 @@
     <t>DEF</t>
   </si>
   <si>
-    <t>TE1</t>
-  </si>
-  <si>
-    <t>TE2</t>
-  </si>
-  <si>
-    <t>TE3</t>
-  </si>
-  <si>
-    <t>TE4</t>
-  </si>
-  <si>
-    <t>TE5</t>
-  </si>
-  <si>
     <t>enddef</t>
   </si>
   <si>
     <t>PPAL</t>
+  </si>
+  <si>
+    <t>Call</t>
+  </si>
+  <si>
+    <t>Tdeffunc</t>
   </si>
   <si>
     <t>endmain</t>
@@ -472,7 +445,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C53"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -601,10 +574,10 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
         <v>19</v>
-      </c>
-      <c r="B12" t="s">
-        <v>20</v>
       </c>
       <c r="C12" t="s">
         <v>12</v>
@@ -612,10 +585,10 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
@@ -623,10 +596,10 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
         <v>12</v>
@@ -634,10 +607,10 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s">
         <v>12</v>
@@ -645,13 +618,13 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17">
@@ -662,7 +635,7 @@
         <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18">
@@ -670,175 +643,175 @@
         <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="C18" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
         <v>28</v>
-      </c>
-      <c r="C19" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="C20" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="C21" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
         <v>23</v>
       </c>
       <c r="C22" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C23" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C24" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" t="s">
         <v>33</v>
-      </c>
-      <c r="C25" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="B26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" t="s">
         <v>34</v>
-      </c>
-      <c r="C26" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="C27" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="C28" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C29" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="C30" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B31" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C31" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B32" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="C32" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B33" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C33" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34">
@@ -849,40 +822,40 @@
         <v>11</v>
       </c>
       <c r="C34" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" t="s">
         <v>37</v>
-      </c>
-      <c r="B35" t="s">
-        <v>38</v>
-      </c>
-      <c r="C35" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="C36" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="B37" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C37" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38">
@@ -893,172 +866,73 @@
         <v>15</v>
       </c>
       <c r="C38" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B39" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C39" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B40" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C40" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="B41" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="C41" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B42" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C42" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B43" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C43" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B44" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C44" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="s">
-        <v>26</v>
-      </c>
-      <c r="B45" t="s">
-        <v>12</v>
-      </c>
-      <c r="C45" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="s">
-        <v>29</v>
-      </c>
-      <c r="B46" t="s">
-        <v>30</v>
-      </c>
-      <c r="C46" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="s">
-        <v>26</v>
-      </c>
-      <c r="B47" t="s">
-        <v>23</v>
-      </c>
-      <c r="C47" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="s">
-        <v>29</v>
-      </c>
-      <c r="B48" t="s">
-        <v>30</v>
-      </c>
-      <c r="C48" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="s">
-        <v>26</v>
-      </c>
-      <c r="B49" t="s">
-        <v>31</v>
-      </c>
-      <c r="C49" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="s">
-        <v>32</v>
-      </c>
-      <c r="B50" t="s">
-        <v>33</v>
-      </c>
-      <c r="C50" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="s">
-        <v>26</v>
-      </c>
-      <c r="B51" t="s">
-        <v>34</v>
-      </c>
-      <c r="C51" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="s">
-        <v>10</v>
-      </c>
-      <c r="B52" t="s">
-        <v>11</v>
-      </c>
-      <c r="C52" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="s">
-        <v>37</v>
-      </c>
-      <c r="B53" t="s">
         <v>38</v>
-      </c>
-      <c r="C53" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1076,16 +950,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -1106,120 +980,120 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
         <v>45</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>47</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>48</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>49</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>50</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>51</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>52</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>53</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>54</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>55</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>56</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>57</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>58</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>59</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>60</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>61</v>
-      </c>
-      <c r="R1" t="s">
-        <v>62</v>
-      </c>
-      <c r="S1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E2" t="s">
-        <v>66</v>
+        <v>32</v>
       </c>
       <c r="F2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="J2" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="K2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="L2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="M2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="N2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="O2" t="s">
         <v>34</v>
       </c>
       <c r="P2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="Q2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="R2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="S2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1237,40 +1111,40 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
       </c>
       <c r="E1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1" t="s">
         <v>71</v>
       </c>
-      <c r="F1" t="s">
+      <c r="K1" t="s">
         <v>72</v>
       </c>
-      <c r="G1" t="s">
+      <c r="L1" t="s">
         <v>73</v>
-      </c>
-      <c r="H1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I1" t="s">
-        <v>75</v>
-      </c>
-      <c r="J1" t="s">
-        <v>76</v>
-      </c>
-      <c r="K1" t="s">
-        <v>77</v>
-      </c>
-      <c r="L1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="2">
@@ -1322,7 +1196,7 @@
         <v>0.0</v>
       </c>
       <c r="D3" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="E3" t="n">
         <v>0.0</v>
@@ -1346,12 +1220,12 @@
         <v>0.0</v>
       </c>
       <c r="L3" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B4" t="n">
         <v>0.0</v>
@@ -1360,7 +1234,7 @@
         <v>0.0</v>
       </c>
       <c r="D4" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="E4" t="n">
         <v>0.0</v>
@@ -1384,7 +1258,7 @@
         <v>0.0</v>
       </c>
       <c r="L4" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
   </sheetData>
@@ -1394,7 +1268,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1405,45 +1279,45 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" t="s">
         <v>80</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I1" t="s">
         <v>81</v>
       </c>
-      <c r="D1" t="s">
+      <c r="J1" t="s">
         <v>82</v>
       </c>
-      <c r="E1" t="s">
+      <c r="K1" t="s">
         <v>83</v>
       </c>
-      <c r="F1" t="s">
+      <c r="L1" t="s">
         <v>84</v>
       </c>
-      <c r="G1" t="s">
+      <c r="M1" t="s">
         <v>85</v>
-      </c>
-      <c r="H1" t="s">
-        <v>83</v>
-      </c>
-      <c r="I1" t="s">
-        <v>86</v>
-      </c>
-      <c r="J1" t="s">
-        <v>87</v>
-      </c>
-      <c r="K1" t="s">
-        <v>88</v>
-      </c>
-      <c r="L1" t="s">
-        <v>89</v>
-      </c>
-      <c r="M1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>3.0</v>
+        <v>7.0</v>
       </c>
       <c r="B2" t="n">
         <v>0.0</v>
@@ -1452,7 +1326,7 @@
         <v>0.0</v>
       </c>
       <c r="D2" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="E2" t="n">
         <v>0.0</v>
@@ -1476,7 +1350,7 @@
         <v>0.0</v>
       </c>
       <c r="L2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="M2" t="n">
         <v>0.0</v>
@@ -1484,7 +1358,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>4.0</v>
+        <v>8.0</v>
       </c>
       <c r="B3" t="n">
         <v>0.0</v>
@@ -1493,7 +1367,7 @@
         <v>0.0</v>
       </c>
       <c r="D3" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E3" t="n">
         <v>0.0</v>
@@ -1517,50 +1391,9 @@
         <v>0.0</v>
       </c>
       <c r="L3" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="M3" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D4" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L4" t="s">
-        <v>91</v>
-      </c>
-      <c r="M4" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1571,7 +1404,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1579,45 +1412,45 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="G1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1130.0</v>
+        <v>1140.0</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C2" t="s">
-        <v>99</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="E2" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="F2" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="G2" t="n">
         <v>1.0</v>
@@ -1625,25 +1458,25 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1090.0</v>
+        <v>1130.0</v>
       </c>
       <c r="B3" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C3" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
       </c>
       <c r="E3" t="n">
-        <v>3.0</v>
+        <v>7.0</v>
       </c>
       <c r="F3" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="G3" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="4">
@@ -1651,88 +1484,88 @@
         <v>1130.0</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E4" t="n">
-        <v>4.0</v>
+        <v>7.0</v>
       </c>
       <c r="F4" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="G4" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1090.0</v>
+        <v>1100.0</v>
       </c>
       <c r="B5" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C5" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E5" t="n">
-        <v>4.0</v>
+        <v>7.0</v>
       </c>
       <c r="F5" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="G5" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1140.0</v>
+        <v>1100.0</v>
       </c>
       <c r="B6" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>94</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="E6" t="n">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
       <c r="F6" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="G6" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1130.0</v>
+        <v>1120.0</v>
       </c>
       <c r="B7" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C7" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E7" t="n">
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
       <c r="F7" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="G7" t="n">
         <v>0.0</v>
@@ -1743,21 +1576,228 @@
         <v>1090.0</v>
       </c>
       <c r="B8" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C8" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
       </c>
       <c r="E8" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1020.0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>93</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>1130.0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" t="s">
+        <v>94</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" t="n">
         <v>8.0</v>
       </c>
-      <c r="F8" t="s">
-        <v>100</v>
-      </c>
-      <c r="G8" t="n">
+      <c r="F10" t="s">
+        <v>93</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>1130.0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>92</v>
+      </c>
+      <c r="C11" t="s">
+        <v>94</v>
+      </c>
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>93</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>1130.0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>92</v>
+      </c>
+      <c r="C12" t="s">
+        <v>94</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>93</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>1100.0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" t="s">
+        <v>94</v>
+      </c>
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="F13" t="s">
+        <v>93</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>1100.0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C14" t="s">
+        <v>94</v>
+      </c>
+      <c r="D14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>93</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>1120.0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>92</v>
+      </c>
+      <c r="C15" t="s">
+        <v>94</v>
+      </c>
+      <c r="D15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="F15" t="s">
+        <v>93</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>1090.0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" t="s">
+        <v>94</v>
+      </c>
+      <c r="D16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>93</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>1020.0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>92</v>
+      </c>
+      <c r="C17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>93</v>
+      </c>
+      <c r="G17" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1776,19 +1816,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1798,7 +1838,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1806,308 +1846,189 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="E1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>92</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>92</v>
       </c>
       <c r="E3" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>92</v>
       </c>
       <c r="E4" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>106</v>
       </c>
       <c r="C5" t="s">
-        <v>111</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>92</v>
       </c>
       <c r="E5" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>92</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>112</v>
+        <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>106</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>92</v>
       </c>
       <c r="E8" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>92</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>98</v>
+        <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B10" t="s">
-        <v>98</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
-        <v>98</v>
+        <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E10" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>92</v>
       </c>
       <c r="C11" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D11" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E11" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" t="s">
-        <v>116</v>
-      </c>
-      <c r="C12" t="s">
-        <v>98</v>
-      </c>
-      <c r="D12" t="s">
-        <v>98</v>
-      </c>
-      <c r="E12" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>98</v>
-      </c>
-      <c r="B13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>98</v>
-      </c>
-      <c r="B14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" t="s">
-        <v>110</v>
-      </c>
-      <c r="D14" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>98</v>
-      </c>
-      <c r="B15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" t="s">
-        <v>111</v>
-      </c>
-      <c r="D15" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>98</v>
-      </c>
-      <c r="B16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" t="s">
-        <v>112</v>
-      </c>
-      <c r="E16" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>98</v>
-      </c>
-      <c r="B17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" t="s">
-        <v>98</v>
-      </c>
-      <c r="E17" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>117</v>
-      </c>
-      <c r="B18" t="s">
-        <v>98</v>
-      </c>
-      <c r="C18" t="s">
-        <v>98</v>
-      </c>
-      <c r="D18" t="s">
-        <v>98</v>
-      </c>
-      <c r="E18" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -2125,79 +2046,79 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1" t="s">
+        <v>82</v>
+      </c>
+      <c r="J1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K1" t="s">
+        <v>114</v>
+      </c>
+      <c r="L1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" t="s">
+        <v>115</v>
+      </c>
+      <c r="N1" t="s">
+        <v>116</v>
+      </c>
+      <c r="O1" t="s">
+        <v>117</v>
+      </c>
+      <c r="P1" t="s">
         <v>118</v>
       </c>
-      <c r="B1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="Q1" t="s">
         <v>119</v>
       </c>
-      <c r="F1" t="s">
+      <c r="R1" t="s">
         <v>120</v>
       </c>
-      <c r="G1" t="s">
-        <v>84</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="S1" t="s">
         <v>121</v>
       </c>
-      <c r="I1" t="s">
-        <v>87</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="T1" t="s">
         <v>122</v>
       </c>
-      <c r="K1" t="s">
+      <c r="U1" t="s">
         <v>123</v>
       </c>
-      <c r="L1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="V1" t="s">
         <v>124</v>
       </c>
-      <c r="N1" t="s">
+      <c r="W1" t="s">
         <v>125</v>
       </c>
-      <c r="O1" t="s">
-        <v>126</v>
-      </c>
-      <c r="P1" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>128</v>
-      </c>
-      <c r="R1" t="s">
-        <v>129</v>
-      </c>
-      <c r="S1" t="s">
-        <v>130</v>
-      </c>
-      <c r="T1" t="s">
-        <v>131</v>
-      </c>
-      <c r="U1" t="s">
-        <v>132</v>
-      </c>
-      <c r="V1" t="s">
-        <v>133</v>
-      </c>
-      <c r="W1" t="s">
-        <v>134</v>
-      </c>
       <c r="X1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="Y1" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2">
@@ -2205,7 +2126,7 @@
         <v>0.0</v>
       </c>
       <c r="B2" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="C2" t="n">
         <v>0.0</v>
@@ -2232,7 +2153,7 @@
         <v>0.0</v>
       </c>
       <c r="K2" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="L2" t="n">
         <v>0.0</v>
@@ -2282,7 +2203,7 @@
         <v>1.0</v>
       </c>
       <c r="B3" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
       <c r="C3" t="n">
         <v>0.0</v>
@@ -2356,10 +2277,10 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="B4" t="n">
-        <v>9.0</v>
+        <v>0.0</v>
       </c>
       <c r="C4" t="n">
         <v>0.0</v>
@@ -2386,7 +2307,7 @@
         <v>0.0</v>
       </c>
       <c r="K4" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="L4" t="n">
         <v>0.0</v>

</xml_diff>